<commit_message>
fix: Update log_respostas.xlsx to reflect recent data changes
</commit_message>
<xml_diff>
--- a/log/log_respostas.xlsx
+++ b/log/log_respostas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Empresa</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>2025-07-17 09:07:27</t>
+  </si>
+  <si>
+    <t>2025-07-17 09:32:01</t>
   </si>
   <si>
     <t>2025-07-17</t>
@@ -455,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,13 +504,13 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -527,13 +530,13 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -553,12 +556,35 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5">
         <v>0</v>
       </c>
     </row>

</xml_diff>